<commit_message>
Changes in Common Folder
</commit_message>
<xml_diff>
--- a/Data Files/Login and Request a Meeting.xlsx
+++ b/Data Files/Login and Request a Meeting.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>url</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>email</t>
   </si>
@@ -48,9 +45,6 @@
   </si>
   <si>
     <t>purpose</t>
-  </si>
-  <si>
-    <t>https://sandbox.vsms.tezzasolutions.com/index</t>
   </si>
   <si>
     <t>dennisgituto1@gmail.com</t>
@@ -439,21 +433,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.44140625" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" customWidth="1"/>
-    <col min="8" max="8" width="27.77734375" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="27.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -475,40 +466,33 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>